<commit_message>
added the elements of water budget (not yet the budget itself)
compute PET, evaporation, transpiration... but does not yet update water content
</commit_message>
<xml_diff>
--- a/exampleinputs/soils.xlsx
+++ b/exampleinputs/soils.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="13600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="275_-45" sheetId="1" r:id="rId1"/>
@@ -109,14 +109,14 @@
     <t>325_-35</t>
   </si>
   <si>
-    <t>VPDcoef</t>
+    <t>VPDF</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -147,6 +147,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -241,7 +248,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -296,6 +303,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
@@ -637,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -699,7 +707,7 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="4"/>
@@ -1071,8 +1079,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1133,7 +1141,7 @@
       <c r="E3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="20" t="s">
         <v>29</v>
       </c>
       <c r="G3" s="4"/>

</xml_diff>